<commit_message>
correction gantt, manque critical path et jalon si on veut mettre
</commit_message>
<xml_diff>
--- a/management/Diagramme de Gantt de projet.xlsx
+++ b/management/Diagramme de Gantt de projet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5F03BC-9457-49DF-90EE-510CC745DC04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601CFE84-85F5-42A4-864F-C035EABD5B30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{568C94E4-E3F7-4EB4-8281-4914A18C47B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{568C94E4-E3F7-4EB4-8281-4914A18C47B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Données du diagramme" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Créez un diagramme de Gantt Suivi de date dans cette feuille de calcul.
 Le titre de cette feuille de calcul figure dans la cellule B1. 
@@ -104,24 +104,6 @@
   </si>
   <si>
     <t>Jalon</t>
-  </si>
-  <si>
-    <t>Jalon 1</t>
-  </si>
-  <si>
-    <t>Jalon 2</t>
-  </si>
-  <si>
-    <t>Jalon 3</t>
-  </si>
-  <si>
-    <t>Jalon 4</t>
-  </si>
-  <si>
-    <t>Jalon 5</t>
-  </si>
-  <si>
-    <t>Jalon 6</t>
   </si>
   <si>
     <t>Tâches</t>
@@ -1317,7 +1299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FF2B7DD-3DC1-4396-A1C9-91D58AE5AB1F}" type="CELLRANGE">
+                    <a:fld id="{8360E003-3A96-4A61-94B3-05A6A9995197}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1350,7 +1332,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83DD0351-56E7-43AE-AB66-45AB38333EEB}" type="CELLRANGE">
+                    <a:fld id="{F62F6801-5D68-4213-906B-DC04AED3A494}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1384,7 +1366,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5547C7F-948B-4804-A18C-70FC50CB8AE6}" type="CELLRANGE">
+                    <a:fld id="{B4AA1CDD-A430-4EE9-8303-E251E3F9AB12}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1418,7 +1400,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5923F182-5A04-4B4B-A566-21C4E0822F13}" type="CELLRANGE">
+                    <a:fld id="{B7E8A714-BDFE-47F2-A9D5-567903DF2195}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1452,7 +1434,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6AA6E12-A33E-437A-A758-E33850D1E4CF}" type="CELLRANGE">
+                    <a:fld id="{0D69365D-731B-4002-84B2-2E61C911FF65}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1486,7 +1468,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{751FDF48-4480-45A5-A44A-BCD53D8EB96D}" type="CELLRANGE">
+                    <a:fld id="{1848BC21-46AD-4C05-9FBF-5395445AAB2D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1520,7 +1502,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B905D61-E3B9-412D-B662-F66BE1C28FF8}" type="CELLRANGE">
+                    <a:fld id="{AD5FB025-1B4E-4A87-91E8-9AD9D465887C}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1603,25 +1585,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>6</c:v>
                   </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>11</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>31</c:v>
-                  </c:pt>
                   <c:pt idx="4">
-                    <c:v>16</c:v>
+                    <c:v>12</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>6</c:v>
+                    <c:v>7</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>3</c:v>
+                    <c:v>7</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1656,25 +1638,25 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>43994</c:v>
+                  <c:v>43978</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43995</c:v>
+                  <c:v>43979</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44002</c:v>
+                  <c:v>43983</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44006</c:v>
+                  <c:v>43980</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44009</c:v>
+                  <c:v>43983</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44019</c:v>
+                  <c:v>43985</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44028</c:v>
+                  <c:v>43987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,25 +1699,25 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>Identifier notre cible</c:v>
+                    <c:v>Créer le slogan</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Fixer notre promesse</c:v>
+                    <c:v>définir notre politique de distribution</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Gestion, cout et rentabilité</c:v>
+                    <c:v>définir notre politique de communication</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Trouver un moyen de faire tester notre produit</c:v>
+                    <c:v>concevoir une identité visuelle attrayante pour le produit</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Créer le slogan</c:v>
+                    <c:v>Survey Editor</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>définir notre politique de distribution</c:v>
+                    <c:v>Data Transfert </c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>définir notre politique de communication</c:v>
+                    <c:v>Survey Analyzer</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1797,7 +1779,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{038BB58B-4B65-4C14-9E79-5A802051735F}" type="CELLRANGE">
+                    <a:fld id="{E486DBC7-6A32-4B9F-ADAB-EDB0CB7F4072}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1100">
@@ -2023,7 +2005,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{743EDDD7-71C5-443A-9428-145FEA9585E0}" type="CELLRANGE">
+                    <a:fld id="{76510760-3881-41F4-98D8-F9F608BC6D65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2056,7 +2038,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FA1615E-2FF9-48DE-8C94-5433701F64DC}" type="CELLRANGE">
+                    <a:fld id="{5C2827CC-1981-4C53-8452-12A71FEAA99B}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2075,7 +2057,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2090,7 +2071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D1948CB-65E2-400E-A4CA-0CB09E22AB63}" type="CELLRANGE">
+                    <a:fld id="{9CEAB5AF-2347-4937-935A-9D65E0D027BA}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2109,7 +2090,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2124,7 +2104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{144B9CAC-1ECD-405C-88DD-04333EA1A783}" type="CELLRANGE">
+                    <a:fld id="{3411930A-9BA6-4073-B90A-ED7F8B430B5F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2143,7 +2123,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2158,7 +2137,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBA04415-EB42-4F11-BCF9-3B149B147584}" type="CELLRANGE">
+                    <a:fld id="{CE51F5F5-F4D6-4AB5-BE8E-DD912C976EC0}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2177,7 +2156,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2192,7 +2170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5E274CA-D24D-4F5D-9B0D-57AC5D3E3A08}" type="CELLRANGE">
+                    <a:fld id="{1C011287-F1A0-466F-9F00-496E01FB18C6}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2211,7 +2189,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2226,7 +2203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99B479D7-27D9-4B25-BA2C-AA58053DCA55}" type="CELLRANGE">
+                    <a:fld id="{97DB082D-EA5C-4AE6-A606-161418147755}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2245,7 +2222,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2260,7 +2236,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{712DDC85-C616-420C-A645-EE4BF0210E5E}" type="CELLRANGE">
+                    <a:fld id="{B5E43203-C24D-4B92-8409-792EB9C1976A}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2279,7 +2255,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2294,7 +2269,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{054E0739-BF70-4BA0-B3CF-8B7B923D3C35}" type="CELLRANGE">
+                    <a:fld id="{62CCF25C-8A40-483E-8D7E-216280A9087E}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2313,7 +2288,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2328,7 +2302,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{046530D4-1D0C-474F-9F49-455FE2ED73D8}" type="CELLRANGE">
+                    <a:fld id="{0A497CD1-DEF0-4492-B429-9BC27C7AAF6F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2347,7 +2321,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2362,7 +2335,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10A4AC6B-64B3-41A3-9EF5-025938D02AB3}" type="CELLRANGE">
+                    <a:fld id="{9D305C95-4DC5-499B-9FEC-9AEEF46073E4}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2381,7 +2354,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2396,7 +2368,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC2FDA9B-F740-42FF-94E9-7CBB12F614A1}" type="CELLRANGE">
+                    <a:fld id="{8FA42799-2122-4681-A912-4D9F2F77F362}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2415,7 +2387,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2430,7 +2401,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9FF03B0-E3B6-4F5C-9E4D-C835EEB7BC1B}" type="CELLRANGE">
+                    <a:fld id="{B8153615-7CC4-46BE-908F-575FF115B987}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2449,7 +2420,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2464,7 +2434,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F3AF8AE-AD03-42B1-85A9-130CB2DBC2CD}" type="CELLRANGE">
+                    <a:fld id="{EA2B1118-C3E1-4933-A861-9B9A2350ECEB}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2483,7 +2453,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2498,7 +2467,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B19C673C-5238-4FFD-AA9D-28E0E3F217ED}" type="CELLRANGE">
+                    <a:fld id="{3523918F-5447-4529-9955-D4C30C7D9BB8}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -2517,7 +2486,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2600,49 +2568,49 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>44003</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44019</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44029</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44038</c:v>
+                  <c:v>43994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2654,13 +2622,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2708,15 +2676,6 @@
                 <c15:f>'Données dynamiques masquées'!$G$18:$G$33</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="16"/>
-                  <c:pt idx="0">
-                    <c:v>Jalon 1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Jalon 2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Jalon 3</c:v>
-                  </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -3410,7 +3369,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="'Données dynamiques masquées'!$B$8" horiz="1" max="100" page="4" val="2"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="'Données dynamiques masquées'!$B$8" horiz="1" max="100" page="4" val="6"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3965,8 +3924,8 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,7 +3971,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4035,21 +3994,21 @@
         <v>9</v>
       </c>
       <c r="H4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>27</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>10</v>
@@ -4067,16 +4026,16 @@
         <v>10</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
         <v>28</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4087,30 +4046,23 @@
       <c r="C6" s="20">
         <v>1</v>
       </c>
-      <c r="D6" s="21">
-        <f ca="1">Date_Début+10</f>
-        <v>44003</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="12"/>
       <c r="G6" s="11">
         <v>1</v>
       </c>
       <c r="H6" s="21">
-        <f ca="1">TODAY()-1</f>
-        <v>43993</v>
+        <v>43969</v>
       </c>
       <c r="I6" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+1</f>
-        <v>43994</v>
+        <v>43970</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K6" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
         <v>2</v>
       </c>
     </row>
@@ -4121,30 +4073,23 @@
       <c r="C7" s="20">
         <v>1</v>
       </c>
-      <c r="D7" s="21">
-        <f ca="1">TODAY()+25</f>
-        <v>44019</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="6"/>
       <c r="G7" s="11">
         <v>2</v>
       </c>
       <c r="H7" s="21">
-        <f ca="1">TODAY()</f>
-        <v>43994</v>
+        <v>43970</v>
       </c>
       <c r="I7" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+1</f>
-        <v>43995</v>
+        <v>43972</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K7" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>2</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -4154,30 +4099,23 @@
       <c r="C8" s="20">
         <v>1</v>
       </c>
-      <c r="D8" s="21">
-        <f ca="1">TODAY()+35</f>
-        <v>44029</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="6"/>
       <c r="G8" s="11">
         <v>3</v>
       </c>
       <c r="H8" s="21">
-        <f ca="1">TODAY()</f>
-        <v>43994</v>
+        <v>43972</v>
       </c>
       <c r="I8" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+5</f>
-        <v>43999</v>
+        <v>43973</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K8" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>6</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -4187,30 +4125,23 @@
       <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="D9" s="21">
-        <f ca="1">TODAY()+45</f>
-        <v>44039</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="6"/>
       <c r="G9" s="11">
         <v>4</v>
       </c>
       <c r="H9" s="22">
-        <f ca="1">TODAY()+1</f>
-        <v>43995</v>
+        <v>43976</v>
       </c>
       <c r="I9" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+7</f>
-        <v>44002</v>
+        <v>43977</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K9" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>8</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -4220,30 +4151,23 @@
       <c r="C10" s="20">
         <v>1</v>
       </c>
-      <c r="D10" s="21">
-        <f ca="1">TODAY()+60</f>
-        <v>44054</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="6"/>
       <c r="G10" s="11">
         <v>5</v>
       </c>
       <c r="H10" s="21">
-        <f ca="1">TODAY()+8</f>
-        <v>44002</v>
+        <v>43971</v>
       </c>
       <c r="I10" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+10</f>
-        <v>44012</v>
+        <v>43973</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="K10" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>11</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4253,30 +4177,23 @@
       <c r="C11" s="20">
         <v>1</v>
       </c>
-      <c r="D11" s="21">
-        <f ca="1">TODAY()+70</f>
-        <v>44064</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="6"/>
       <c r="G11" s="11">
         <v>6</v>
       </c>
       <c r="H11" s="21">
-        <f ca="1">TODAY()+12</f>
-        <v>44006</v>
+        <v>43976</v>
       </c>
       <c r="I11" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+30</f>
-        <v>44036</v>
+        <v>43977</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="K11" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>31</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -4288,19 +4205,17 @@
         <v>7</v>
       </c>
       <c r="H12" s="21">
-        <f ca="1">TODAY()+15</f>
-        <v>44009</v>
+        <v>43978</v>
       </c>
       <c r="I12" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+15</f>
-        <v>44024</v>
+        <v>43979</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K12" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>16</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4312,19 +4227,17 @@
         <v>8</v>
       </c>
       <c r="H13" s="21">
-        <f ca="1">TODAY()+25</f>
-        <v>44019</v>
+        <v>43979</v>
       </c>
       <c r="I13" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+5</f>
-        <v>44024</v>
+        <v>43980</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K13" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>6</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4336,18 +4249,16 @@
         <v>9</v>
       </c>
       <c r="H14" s="21">
-        <f ca="1">TODAY()+34</f>
-        <v>44028</v>
+        <v>43983</v>
       </c>
       <c r="I14" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+2</f>
-        <v>44030</v>
+        <v>43985</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K14" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
         <v>3</v>
       </c>
     </row>
@@ -4360,19 +4271,17 @@
         <v>10</v>
       </c>
       <c r="H15" s="21">
-        <f ca="1">TODAY()+40</f>
-        <v>44034</v>
+        <v>43980</v>
       </c>
       <c r="I15" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+30</f>
-        <v>44064</v>
+        <v>43985</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K15" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>31</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -4384,19 +4293,17 @@
         <v>11</v>
       </c>
       <c r="H16" s="21">
-        <f ca="1">TODAY()+42</f>
-        <v>44036</v>
+        <v>43983</v>
       </c>
       <c r="I16" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+23</f>
-        <v>44059</v>
+        <v>43994</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K16" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>24</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -4408,19 +4315,17 @@
         <v>12</v>
       </c>
       <c r="H17" s="21">
-        <f ca="1">TODAY()+50</f>
-        <v>44044</v>
+        <v>43985</v>
       </c>
       <c r="I17" s="21">
-        <f ca="1">Tâches[[#This Row],[Date de début]]+5</f>
-        <v>44049</v>
+        <v>43991</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K17" s="24">
-        <f ca="1">IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>6</v>
+        <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -4432,17 +4337,17 @@
         <v>13</v>
       </c>
       <c r="H18" s="21">
-        <v>44053</v>
+        <v>43987</v>
       </c>
       <c r="I18" s="21">
-        <v>44057</v>
+        <v>43993</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K18" s="24">
         <f>IFERROR(IF(LEN(Tâches[[#This Row],[Date de début]])=0,"",(INT(Tâches[[#This Row],[Date de fin]])-INT(Tâches[[#This Row],[Date de début]]))-(INT(Tâches[[#This Row],[Date de début]])-INT(Tâches[[#This Row],[Date de début]]))+1),"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -4537,7 +4442,7 @@
         <v>5</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -4572,8 +4477,8 @@
   </sheetPr>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4587,7 +4492,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -4678,33 +4583,33 @@
   <sheetData>
     <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="str">
         <f ca="1">IF(TODAY()&gt;=MIN(DonnéesTâcheDynamiques[Date de début]),"Aujourd’hui","")</f>
         <v>Aujourd’hui</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4732,15 +4637,15 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4748,19 +4653,19 @@
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <f ca="1">IFERROR(IF(IncrémentDéfilement[incrément de défilement]=0,Date_Début,IF(Date_Début+IncrémentDéfilement[incrément de défilement]*15&lt;Date_Fin,Date_Début+IncrémentDéfilement[incrément de défilement]*15,Date_Fin-1)),"")</f>
-        <v>44023</v>
+        <v>43993</v>
       </c>
       <c r="D11">
         <v>45</v>
@@ -4769,41 +4674,41 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f ca="1">IFERROR(IF($B$11+15&lt;Date_Fin,$B$11+15,Date_Fin),"")</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Données du diagramme'!$H6,IncrémentDéfilement[incrément de défilement],0,1,1))=0,"",IF(OR(OFFSET('Données du diagramme'!$I6,IncrémentDéfilement[incrément de défilement],0,1,1)&lt;=$B$12,OFFSET('Données du diagramme'!$H6,IncrémentDéfilement[incrément de défilement],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tâches[],OFFSET('Données du diagramme'!$G6,IncrémentDéfilement[incrément de défilement],0,1,1),4),"")),"")</f>
-        <v>Identifier notre cible</v>
+        <v>Créer le slogan</v>
       </c>
       <c r="C15" s="23">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,$B$11,INDEX(Tâches[],OFFSET('Données du diagramme'!$G6,IncrémentDéfilement[incrément de défilement],0,1,1),2)),"")</f>
-        <v>43994</v>
+        <v>43978</v>
       </c>
       <c r="D15" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,0,IF(AND('Données du diagramme'!$H6&lt;=$B$12,'Données du diagramme'!$I6&gt;=$B$12),ABS(OFFSET('Données du diagramme'!$H6,IncrémentDéfilement[incrément de défilement],0,1,1)-$B$12)+1,OFFSET('Données du diagramme'!$K6,IncrémentDéfilement[incrément de défilement],0,1,1))),"")</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,"",8),"")</f>
@@ -4813,39 +4718,39 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Données du diagramme'!$H7,IncrémentDéfilement[incrément de défilement],0,1,1))=0,"",IF(OR(OFFSET('Données du diagramme'!$I7,IncrémentDéfilement[incrément de défilement],0,1,1)&lt;=$B$12,OFFSET('Données du diagramme'!$H7,IncrémentDéfilement[incrément de défilement],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tâches[],OFFSET('Données du diagramme'!$G7,IncrémentDéfilement[incrément de défilement],0,1,1),4),"")),"")</f>
-        <v>Fixer notre promesse</v>
+        <v>définir notre politique de distribution</v>
       </c>
       <c r="C16" s="23">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,$B$11,INDEX(Tâches[],OFFSET('Données du diagramme'!$G7,IncrémentDéfilement[incrément de défilement],0,1,1),2)),"")</f>
-        <v>43995</v>
+        <v>43979</v>
       </c>
       <c r="D16" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,0,IF(AND('Données du diagramme'!$H7&lt;=$B$12,'Données du diagramme'!$I7&gt;=$B$12),ABS(OFFSET('Données du diagramme'!$H7,IncrémentDéfilement[incrément de défilement],0,1,1)-$B$12)+1,OFFSET('Données du diagramme'!$K7,IncrémentDéfilement[incrément de défilement],0,1,1))),"")</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E16" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,"",7),"")</f>
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Données du diagramme'!$H8,IncrémentDéfilement[incrément de défilement],0,1,1))=0,"",IF(OR(OFFSET('Données du diagramme'!$I8,IncrémentDéfilement[incrément de défilement],0,1,1)&lt;=$B$12,OFFSET('Données du diagramme'!$H8,IncrémentDéfilement[incrément de défilement],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tâches[],OFFSET('Données du diagramme'!$G8,IncrémentDéfilement[incrément de défilement],0,1,1),4),"")),"")</f>
-        <v>Gestion, cout et rentabilité</v>
+        <v>définir notre politique de communication</v>
       </c>
       <c r="C17" s="23">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,$B$11,INDEX(Tâches[],OFFSET('Données du diagramme'!$G8,IncrémentDéfilement[incrément de défilement],0,1,1),2)),"")</f>
-        <v>44002</v>
+        <v>43983</v>
       </c>
       <c r="D17" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,0,IF(AND('Données du diagramme'!$H8&lt;=$B$12,'Données du diagramme'!$I8&gt;=$B$12),ABS(OFFSET('Données du diagramme'!$H8,IncrémentDéfilement[incrément de défilement],0,1,1)-$B$12)+1,OFFSET('Données du diagramme'!$K8,IncrémentDéfilement[incrément de défilement],0,1,1))),"")</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E17" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,"",6),"")</f>
@@ -4855,160 +4760,160 @@
         <v>8</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Données du diagramme'!$H9,IncrémentDéfilement[incrément de défilement],0,1,1))=0,"",IF(OR(OFFSET('Données du diagramme'!$I9,IncrémentDéfilement[incrément de défilement],0,1,1)&lt;=$B$12,OFFSET('Données du diagramme'!$H9,IncrémentDéfilement[incrément de défilement],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tâches[],OFFSET('Données du diagramme'!$G9,IncrémentDéfilement[incrément de défilement],0,1,1),4),"")),"")</f>
-        <v>Trouver un moyen de faire tester notre produit</v>
+        <v>concevoir une identité visuelle attrayante pour le produit</v>
       </c>
       <c r="C18" s="23">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,$B$11,INDEX(Tâches[],OFFSET('Données du diagramme'!$G9,IncrémentDéfilement[incrément de défilement],0,1,1),2)),"")</f>
-        <v>44006</v>
+        <v>43980</v>
       </c>
       <c r="D18" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,0,IF(AND('Données du diagramme'!$H9&lt;=$B$12,'Données du diagramme'!$I9&gt;=$B$12),ABS(OFFSET('Données du diagramme'!$H9,IncrémentDéfilement[incrément de défilement],0,1,1)-$B$12)+1,OFFSET('Données du diagramme'!$K9,IncrémentDéfilement[incrément de défilement],0,1,1))),"")</f>
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E18" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,"",5),"")</f>
         <v>5</v>
       </c>
       <c r="G18" s="7" t="str">
-        <f ca="1">IFERROR(IF(LEN('Données du diagramme'!D6)=0,"",IF(AND('Données du diagramme'!D6&lt;=$B$12,'Données du diagramme'!D6&gt;=$B$11-$D$11),'Données du diagramme'!E6,"")),"")</f>
-        <v>Jalon 1</v>
+        <f>IFERROR(IF(LEN('Données du diagramme'!D6)=0,"",IF(AND('Données du diagramme'!D6&lt;=$B$12,'Données du diagramme'!D6&gt;=$B$11-$D$11),'Données du diagramme'!E6,"")),"")</f>
+        <v/>
       </c>
       <c r="H18" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D6),2)</f>
-        <v>44003</v>
-      </c>
-      <c r="I18" s="8">
-        <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C6),"")</f>
-        <v>1</v>
+        <v>43994</v>
+      </c>
+      <c r="I18" s="8" t="str">
+        <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C6),"")</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Données du diagramme'!$H10,IncrémentDéfilement[incrément de défilement],0,1,1))=0,"",IF(OR(OFFSET('Données du diagramme'!$I10,IncrémentDéfilement[incrément de défilement],0,1,1)&lt;=$B$12,OFFSET('Données du diagramme'!$H10,IncrémentDéfilement[incrément de défilement],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tâches[],OFFSET('Données du diagramme'!$G10,IncrémentDéfilement[incrément de défilement],0,1,1),4),"")),"")</f>
-        <v>Créer le slogan</v>
+        <v>Survey Editor</v>
       </c>
       <c r="C19" s="23">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,$B$11,INDEX(Tâches[],OFFSET('Données du diagramme'!$G10,IncrémentDéfilement[incrément de défilement],0,1,1),2)),"")</f>
-        <v>44009</v>
+        <v>43983</v>
       </c>
       <c r="D19" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,0,IF(AND('Données du diagramme'!$H10&lt;=$B$12,'Données du diagramme'!$I10&gt;=$B$12),ABS(OFFSET('Données du diagramme'!$H10,IncrémentDéfilement[incrément de défilement],0,1,1)-$B$12)+1,OFFSET('Données du diagramme'!$K10,IncrémentDéfilement[incrément de défilement],0,1,1))),"")</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E19" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,"",4),"")</f>
         <v>4</v>
       </c>
       <c r="G19" s="7" t="str">
-        <f ca="1">IFERROR(IF(LEN('Données du diagramme'!D7)=0,"",IF(AND('Données du diagramme'!D7&lt;=$B$12,'Données du diagramme'!D7&gt;=$B$11-$D$11),'Données du diagramme'!E7,"")),"")</f>
-        <v>Jalon 2</v>
+        <f>IFERROR(IF(LEN('Données du diagramme'!D7)=0,"",IF(AND('Données du diagramme'!D7&lt;=$B$12,'Données du diagramme'!D7&gt;=$B$11-$D$11),'Données du diagramme'!E7,"")),"")</f>
+        <v/>
       </c>
       <c r="H19" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D7),2)</f>
-        <v>44019</v>
-      </c>
-      <c r="I19" s="8">
-        <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C7),"")</f>
-        <v>1</v>
+        <v>43994</v>
+      </c>
+      <c r="I19" s="8" t="str">
+        <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C7),"")</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Données du diagramme'!$H11,IncrémentDéfilement[incrément de défilement],0,1,1))=0,"",IF(OR(OFFSET('Données du diagramme'!$I11,IncrémentDéfilement[incrément de défilement],0,1,1)&lt;=$B$12,OFFSET('Données du diagramme'!$H11,IncrémentDéfilement[incrément de défilement],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tâches[],OFFSET('Données du diagramme'!$G11,IncrémentDéfilement[incrément de défilement],0,1,1),4),"")),"")</f>
-        <v>définir notre politique de distribution</v>
+        <v xml:space="preserve">Data Transfert </v>
       </c>
       <c r="C20" s="23">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,$B$11,INDEX(Tâches[],OFFSET('Données du diagramme'!$G11,IncrémentDéfilement[incrément de défilement],0,1,1),2)),"")</f>
-        <v>44019</v>
+        <v>43985</v>
       </c>
       <c r="D20" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,0,IF(AND('Données du diagramme'!$H11&lt;=$B$12,'Données du diagramme'!$I11&gt;=$B$12),ABS(OFFSET('Données du diagramme'!$H11,IncrémentDéfilement[incrément de défilement],0,1,1)-$B$12)+1,OFFSET('Données du diagramme'!$K11,IncrémentDéfilement[incrément de défilement],0,1,1))),"")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E20" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,"",3),"")</f>
         <v>3</v>
       </c>
       <c r="G20" s="7" t="str">
-        <f ca="1">IFERROR(IF(LEN('Données du diagramme'!D8)=0,"",IF(AND('Données du diagramme'!D8&lt;=$B$12,'Données du diagramme'!D8&gt;=$B$11-$D$11),'Données du diagramme'!E8,"")),"")</f>
-        <v>Jalon 3</v>
+        <f>IFERROR(IF(LEN('Données du diagramme'!D8)=0,"",IF(AND('Données du diagramme'!D8&lt;=$B$12,'Données du diagramme'!D8&gt;=$B$11-$D$11),'Données du diagramme'!E8,"")),"")</f>
+        <v/>
       </c>
       <c r="H20" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D8),2)</f>
-        <v>44029</v>
-      </c>
-      <c r="I20" s="8">
-        <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C8),"")</f>
-        <v>1</v>
+        <v>43994</v>
+      </c>
+      <c r="I20" s="8" t="str">
+        <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C8),"")</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Données du diagramme'!$H12,IncrémentDéfilement[incrément de défilement],0,1,1))=0,"",IF(OR(OFFSET('Données du diagramme'!$I12,IncrémentDéfilement[incrément de défilement],0,1,1)&lt;=$B$12,OFFSET('Données du diagramme'!$H12,IncrémentDéfilement[incrément de défilement],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tâches[],OFFSET('Données du diagramme'!$G12,IncrémentDéfilement[incrément de défilement],0,1,1),4),"")),"")</f>
-        <v>définir notre politique de communication</v>
+        <v>Survey Analyzer</v>
       </c>
       <c r="C21" s="23">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,$B$11,INDEX(Tâches[],OFFSET('Données du diagramme'!$G12,IncrémentDéfilement[incrément de défilement],0,1,1),2)),"")</f>
-        <v>44028</v>
+        <v>43987</v>
       </c>
       <c r="D21" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,0,IF(AND('Données du diagramme'!$H12&lt;=$B$12,'Données du diagramme'!$I12&gt;=$B$12),ABS(OFFSET('Données du diagramme'!$H12,IncrémentDéfilement[incrément de défilement],0,1,1)-$B$12)+1,OFFSET('Données du diagramme'!$K12,IncrémentDéfilement[incrément de défilement],0,1,1))),"")</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E21" s="3">
         <f ca="1">IFERROR(IF(LEN(DonnéesTâcheDynamiques[[#This Row],[Tâches]])=0,"",2),"")</f>
         <v>2</v>
       </c>
       <c r="G21" s="7" t="str">
-        <f ca="1">IFERROR(IF(LEN('Données du diagramme'!D9)=0,"",IF(AND('Données du diagramme'!D9&lt;=$B$12,'Données du diagramme'!D9&gt;=$B$11-$D$11),'Données du diagramme'!E9,"")),"")</f>
+        <f>IFERROR(IF(LEN('Données du diagramme'!D9)=0,"",IF(AND('Données du diagramme'!D9&lt;=$B$12,'Données du diagramme'!D9&gt;=$B$11-$D$11),'Données du diagramme'!E9,"")),"")</f>
         <v/>
       </c>
       <c r="H21" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D9),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I21" s="8" t="str">
-        <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C9),"")</f>
+        <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C9),"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22" s="7" t="str">
-        <f ca="1">IFERROR(IF(LEN('Données du diagramme'!D10)=0,"",IF(AND('Données du diagramme'!D10&lt;=$B$12,'Données du diagramme'!D10&gt;=$B$11-$D$11),'Données du diagramme'!E10,"")),"")</f>
+        <f>IFERROR(IF(LEN('Données du diagramme'!D10)=0,"",IF(AND('Données du diagramme'!D10&lt;=$B$12,'Données du diagramme'!D10&gt;=$B$11-$D$11),'Données du diagramme'!E10,"")),"")</f>
         <v/>
       </c>
       <c r="H22" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D10),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I22" s="8" t="str">
-        <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C10),"")</f>
+        <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C10),"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G23" s="7" t="str">
-        <f ca="1">IFERROR(IF(LEN('Données du diagramme'!D11)=0,"",IF(AND('Données du diagramme'!D11&lt;=$B$12,'Données du diagramme'!D11&gt;=$B$11-$D$11),'Données du diagramme'!E11,"")),"")</f>
+        <f>IFERROR(IF(LEN('Données du diagramme'!D11)=0,"",IF(AND('Données du diagramme'!D11&lt;=$B$12,'Données du diagramme'!D11&gt;=$B$11-$D$11),'Données du diagramme'!E11,"")),"")</f>
         <v/>
       </c>
       <c r="H23" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D11),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I23" s="8" t="str">
-        <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C11),"")</f>
+        <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C11),"")</f>
         <v/>
       </c>
     </row>
@@ -5019,7 +4924,7 @@
       </c>
       <c r="H24" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D12),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I24" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C12),"")</f>
@@ -5033,7 +4938,7 @@
       </c>
       <c r="H25" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D13),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I25" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C13),"")</f>
@@ -5047,7 +4952,7 @@
       </c>
       <c r="H26" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D14),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I26" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C14),"")</f>
@@ -5061,7 +4966,7 @@
       </c>
       <c r="H27" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D15),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I27" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C15),"")</f>
@@ -5075,7 +4980,7 @@
       </c>
       <c r="H28" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D16),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I28" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C16),"")</f>
@@ -5089,7 +4994,7 @@
       </c>
       <c r="H29" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D17),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I29" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C17),"")</f>
@@ -5103,7 +5008,7 @@
       </c>
       <c r="H30" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D18),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I30" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C18),"")</f>
@@ -5117,7 +5022,7 @@
       </c>
       <c r="H31" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D19),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I31" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C19),"")</f>
@@ -5126,7 +5031,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G32" s="7" t="str">
         <f>IFERROR(IF(LEN('Données du diagramme'!D20)=0,"",IF(AND('Données du diagramme'!D20&lt;=$B$12,'Données du diagramme'!D20&gt;=$B$11-$D$11),'Données du diagramme'!E20,"")),"")</f>
@@ -5134,14 +5039,14 @@
       </c>
       <c r="H32" s="21">
         <f ca="1">IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,$B$12,'Données du diagramme'!$D20),2)</f>
-        <v>44038</v>
+        <v>43994</v>
       </c>
       <c r="I32" s="8" t="str">
         <f>IFERROR(IF(LEN(DonnéesJalonDynamiques[[#This Row],[Jalons]])=0,"",'Données du diagramme'!$C20),"")</f>
         <v/>
       </c>
       <c r="J32" s="12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -5181,57 +5086,57 @@
   <sheetData>
     <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>